<commit_message>
live window working but messages not coming after the window is closed
</commit_message>
<xml_diff>
--- a/multiple_profiles_sorted_results.xlsx
+++ b/multiple_profiles_sorted_results.xlsx
@@ -473,113 +473,113 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_1-Wind_1-ESS_1</t>
+          <t>IPP241-Solar_3-Wind_1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>103.099190244392</v>
+        <v>129.7316043227053</v>
       </c>
       <c r="C2" t="n">
-        <v>99.64452975237265</v>
+        <v>88.24017042041037</v>
       </c>
       <c r="D2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3389.959170067472</v>
+        <v>3164.081687917208</v>
       </c>
       <c r="F2" t="n">
-        <v>4389.959170067472</v>
+        <v>4164.081687917208</v>
       </c>
       <c r="G2" t="n">
-        <v>65.00000000011937</v>
+        <v>65.00000000011914</v>
       </c>
       <c r="H2" t="n">
-        <v>13.50218545543646</v>
+        <v>17.64700479759088</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_2-Wind_1-ESS_1</t>
+          <t>IPP241-Solar_3-Wind_6</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>98.68936793756286</v>
+        <v>133.1287247831341</v>
       </c>
       <c r="C3" t="n">
-        <v>102.0432121092483</v>
+        <v>87.03541073781425</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3439.964602686343</v>
+        <v>3220.761226087495</v>
       </c>
       <c r="F3" t="n">
-        <v>4439.964602686343</v>
+        <v>4220.761226087495</v>
       </c>
       <c r="G3" t="n">
-        <v>65.00000000011961</v>
+        <v>65.00000000011914</v>
       </c>
       <c r="H3" t="n">
-        <v>13.02590946731322</v>
+        <v>18.25556568411022</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_1-Wind_2-ESS_1</t>
+          <t>IPP241-Solar_4-Wind_1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>200</v>
+        <v>103.099190244392</v>
       </c>
       <c r="C4" t="n">
-        <v>63.78080022266836</v>
+        <v>99.64452975237268</v>
       </c>
       <c r="D4" t="n">
-        <v>37.4172212383823</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>3807.014872210519</v>
+        <v>3389.959170067466</v>
       </c>
       <c r="F4" t="n">
-        <v>4807.014872210519</v>
+        <v>4389.959170067466</v>
       </c>
       <c r="G4" t="n">
-        <v>65.00000000011929</v>
+        <v>65.00000000011939</v>
       </c>
       <c r="H4" t="n">
-        <v>27.34555967856782</v>
+        <v>13.50218545543646</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_2-Wind_2-ESS_1</t>
+          <t>IPP241-Solar_4-Wind_6</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>130</v>
+        <v>106.191019047453</v>
       </c>
       <c r="C5" t="n">
-        <v>79.27929399581578</v>
+        <v>98.05969899680531</v>
       </c>
       <c r="D5" t="n">
-        <v>59.53383606904863</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>4165.696458258275</v>
+        <v>3453.868883793133</v>
       </c>
       <c r="F5" t="n">
-        <v>5165.696458258275</v>
+        <v>4453.868883793133</v>
       </c>
       <c r="G5" t="n">
-        <v>65.00000000011924</v>
+        <v>65.0000000001194</v>
       </c>
       <c r="H5" t="n">
-        <v>11.29879909335846</v>
+        <v>13.87958373221947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everything working till now
</commit_message>
<xml_diff>
--- a/multiple_profiles_sorted_results.xlsx
+++ b/multiple_profiles_sorted_results.xlsx
@@ -483,69 +483,69 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Wind_1-ESS_1</t>
+          <t>IPP369-Wind_1-ESS_1</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.974942838377783</v>
+        <v>110.2263153116867</v>
       </c>
       <c r="D2" t="n">
-        <v>140.0698733936311</v>
+        <v>35.17716761216561</v>
       </c>
       <c r="E2" t="n">
-        <v>4561.471510775326</v>
+        <v>7912.102334764987</v>
       </c>
       <c r="F2" t="n">
-        <v>5561.471510775326</v>
+        <v>8912.102334764986</v>
       </c>
       <c r="G2" t="n">
-        <v>31059532.08531777</v>
+        <v>1473690210.906502</v>
       </c>
       <c r="H2" t="n">
-        <v>65.00000000000013</v>
+        <v>64.99999999999994</v>
       </c>
       <c r="I2" t="n">
-        <v>6809.103600000013</v>
+        <v>186257.7287999998</v>
       </c>
       <c r="J2" t="n">
-        <v>1.489598972978839</v>
+        <v>30.000000000019</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Wind_1-ESS_2</t>
+          <t>IPP369-Wind_1-ESS_2</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.974942838377783</v>
+        <v>95.99196815140722</v>
       </c>
       <c r="D3" t="n">
-        <v>140.0698733936311</v>
+        <v>53.15942122632188</v>
       </c>
       <c r="E3" t="n">
-        <v>4561.471510775326</v>
+        <v>9115.783038975145</v>
       </c>
       <c r="F3" t="n">
-        <v>5561.471510775326</v>
+        <v>10115.78303897515</v>
       </c>
       <c r="G3" t="n">
-        <v>31059532.08531777</v>
+        <v>1697885045.07307</v>
       </c>
       <c r="H3" t="n">
-        <v>65.00000000000013</v>
+        <v>64.99999999999991</v>
       </c>
       <c r="I3" t="n">
-        <v>6809.103600000013</v>
+        <v>186257.7287999997</v>
       </c>
       <c r="J3" t="n">
-        <v>1.489598972978839</v>
+        <v>30.00000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
powerx model done, scheduling left
</commit_message>
<xml_diff>
--- a/multiple_profiles_sorted_results.xlsx
+++ b/multiple_profiles_sorted_results.xlsx
@@ -487,167 +487,167 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27.58420217684733</v>
+        <v>4.135063959726197</v>
       </c>
       <c r="C2" t="n">
-        <v>49.53560416003003</v>
+        <v>29.9736666399491</v>
       </c>
       <c r="D2" t="n">
-        <v>52.61740812351554</v>
+        <v>18.75697678820473</v>
       </c>
       <c r="E2" t="n">
-        <v>9651.815383804371</v>
+        <v>9506.750456525891</v>
       </c>
       <c r="F2" t="n">
-        <v>10651.81538380437</v>
+        <v>10506.75045652589</v>
       </c>
       <c r="G2" t="n">
-        <v>1501125045.122499</v>
+        <v>596223854.8115311</v>
       </c>
       <c r="H2" t="n">
-        <v>64.99999999999976</v>
+        <v>65.00000000000007</v>
       </c>
       <c r="I2" t="n">
-        <v>155527.7411999994</v>
+        <v>62715.84150000006</v>
       </c>
       <c r="J2" t="n">
-        <v>26.45724893107394</v>
+        <v>30.00000000001278</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_2-Wind_1-ESS_2</t>
+          <t>IPP585-Solar_1-Wind_1-ESS_2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>110</v>
+        <v>73.6457638928412</v>
       </c>
       <c r="C3" t="n">
         <v>-0</v>
       </c>
       <c r="D3" t="n">
-        <v>169.5293505172751</v>
+        <v>96.32362176882462</v>
       </c>
       <c r="E3" t="n">
-        <v>23925.05623954744</v>
+        <v>34335.64260191843</v>
       </c>
       <c r="F3" t="n">
-        <v>24925.05623954744</v>
+        <v>35335.64260191843</v>
       </c>
       <c r="G3" t="n">
-        <v>3721009955.019769</v>
+        <v>2153388719.222576</v>
       </c>
       <c r="H3" t="n">
-        <v>64.9999999999998</v>
+        <v>65.00000000000037</v>
       </c>
       <c r="I3" t="n">
-        <v>155527.7411999995</v>
+        <v>62715.84150000035</v>
       </c>
       <c r="J3" t="n">
-        <v>26.91873243673608</v>
+        <v>30.00000000003407</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_2-Wind_2-ESS_2</t>
+          <t>IPP585-Solar_1-Wind_2-ESS_2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>110</v>
+        <v>73.6457638928412</v>
       </c>
       <c r="C4" t="n">
         <v>-0</v>
       </c>
       <c r="D4" t="n">
-        <v>169.5293505172751</v>
+        <v>96.32362176882462</v>
       </c>
       <c r="E4" t="n">
-        <v>23925.05623954744</v>
+        <v>34335.64260191843</v>
       </c>
       <c r="F4" t="n">
-        <v>24925.05623954744</v>
+        <v>35335.64260191843</v>
       </c>
       <c r="G4" t="n">
-        <v>3721009955.019769</v>
+        <v>2153388719.222576</v>
       </c>
       <c r="H4" t="n">
-        <v>64.9999999999998</v>
+        <v>65.00000000000037</v>
       </c>
       <c r="I4" t="n">
-        <v>155527.7411999995</v>
+        <v>62715.84150000035</v>
       </c>
       <c r="J4" t="n">
-        <v>26.91873243673608</v>
+        <v>30.00000000003407</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_1-Wind_1-ESS_2</t>
+          <t>IPP585-Solar_2-Wind_1-ESS_2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>186.0698867343974</v>
+        <v>72.01408538931113</v>
       </c>
       <c r="C5" t="n">
         <v>-0</v>
       </c>
       <c r="D5" t="n">
-        <v>148.0493368312261</v>
+        <v>97.97904427143409</v>
       </c>
       <c r="E5" t="n">
-        <v>23954.89202789721</v>
+        <v>35101.2384516903</v>
       </c>
       <c r="F5" t="n">
-        <v>24954.89202789721</v>
+        <v>36101.2384516903</v>
       </c>
       <c r="G5" t="n">
-        <v>3725650247.788759</v>
+        <v>2201403707.189928</v>
       </c>
       <c r="H5" t="n">
-        <v>65.00000000000034</v>
+        <v>65.0000000000004</v>
       </c>
       <c r="I5" t="n">
-        <v>155527.7412000008</v>
+        <v>62715.84150000038</v>
       </c>
       <c r="J5" t="n">
-        <v>30.00000000003452</v>
+        <v>30.00000000001602</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>IPP585-Solar_1-Wind_2-ESS_2</t>
+          <t>IPP585-Solar_2-Wind_2-ESS_2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>186.0698867343974</v>
+        <v>72.01408538931113</v>
       </c>
       <c r="C6" t="n">
         <v>-0</v>
       </c>
       <c r="D6" t="n">
-        <v>148.0493368312261</v>
+        <v>97.97904427143409</v>
       </c>
       <c r="E6" t="n">
-        <v>23954.89202789721</v>
+        <v>35101.2384516903</v>
       </c>
       <c r="F6" t="n">
-        <v>24954.89202789721</v>
+        <v>36101.2384516903</v>
       </c>
       <c r="G6" t="n">
-        <v>3725650247.788759</v>
+        <v>2201403707.189928</v>
       </c>
       <c r="H6" t="n">
-        <v>65.00000000000034</v>
+        <v>65.0000000000004</v>
       </c>
       <c r="I6" t="n">
-        <v>155527.7412000008</v>
+        <v>62715.84150000038</v>
       </c>
       <c r="J6" t="n">
-        <v>30.00000000003452</v>
+        <v>30.00000000001602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>